<commit_message>
adjust the protocol doc
</commit_message>
<xml_diff>
--- a/messagetemplates/2016NewVersion/BussinessProtoDesign.xlsx
+++ b/messagetemplates/2016NewVersion/BussinessProtoDesign.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>消息名</t>
   </si>
@@ -27,58 +27,201 @@
     <t>字段名</t>
   </si>
   <si>
-    <t>内容</t>
-  </si>
-  <si>
     <t>任务下达</t>
   </si>
   <si>
+    <t>任务下达回文</t>
+  </si>
+  <si>
+    <t>任务状态汇报</t>
+  </si>
+  <si>
+    <t>资源列表查询回文</t>
+  </si>
+  <si>
+    <t>状态查询回文</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>含义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taskid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resources</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>executor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list&lt;string&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>任务ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>资源列表</t>
-  </si>
-  <si>
-    <t>处理用的docker</t>
-  </si>
-  <si>
-    <t>任务下达回文</t>
-  </si>
-  <si>
-    <t>任务状态汇报</t>
-  </si>
-  <si>
-    <t>资源列表查询</t>
-  </si>
-  <si>
-    <t>资源列表查询回文</t>
-  </si>
-  <si>
-    <t>状态查询</t>
-  </si>
-  <si>
-    <t>状态查询回文</t>
-  </si>
-  <si>
-    <t>类型</t>
-  </si>
-  <si>
-    <t>参数</t>
-  </si>
-  <si>
-    <t>结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结果目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taskid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0为成功，&gt;0失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>失败原因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为空则返回所有任务状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list&lt;string&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servant列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servants</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行器列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servantid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpu核心数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>memory数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size_t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size_t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0为正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -102,11 +245,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -122,7 +271,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -384,91 +533,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="28.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>